<commit_message>
fix: remove all OnlyFans banned words from scripts, XLSX, and HTML guides
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/marco/Marco_Complete_Infloww.xlsx
+++ b/marco/Marco_Complete_Infloww.xlsx
@@ -862,7 +862,7 @@
       </c>
       <c r="B18" s="5" t="inlineStr">
         <is>
-          <t>I'm hard and I can't do shit about it because of you</t>
+          <t>I'm hard and I can't do anything about it because of you</t>
         </is>
       </c>
       <c r="C18" s="5" t="inlineStr"/>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="B31" s="8" t="inlineStr">
         <is>
-          <t>gotta say... talking to you is different. most guys on here bore me to death</t>
+          <t>gotta say... talking to you is different. most guys on here are so boring honestly</t>
         </is>
       </c>
       <c r="C31" s="8" t="inlineStr">
@@ -1139,7 +1139,7 @@
       </c>
       <c r="B35" s="8" t="inlineStr">
         <is>
-          <t>hey man, nice to meet you. so what made you hit subscribe?</t>
+          <t>hey man, glad you're here. so what made you hit subscribe?</t>
         </is>
       </c>
       <c r="C35" s="8" t="inlineStr">
@@ -4316,7 +4316,7 @@
       </c>
       <c r="B6" s="13" t="inlineStr">
         <is>
-          <t>holy shit that is... fuck. I need to show you something right now</t>
+          <t>oh fuck that is... damn. I need to show you something right now</t>
         </is>
       </c>
       <c r="C6" s="13" t="inlineStr">

</xml_diff>